<commit_message>
Implemented saving the threshold in the model
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Education\Master\Machine learning in applications\mla-prj-23-zomm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B94E3A-7B0C-4BD1-B625-9A543DE7AB1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880ECAF8-B67D-46B9-9236-2958A5DF7FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8B416CC3-3AED-4146-89A3-0A909EA57107}"/>
   </bookViews>
@@ -103,7 +103,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -341,6 +341,19 @@
         <color indexed="64"/>
       </left>
       <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -353,37 +366,62 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -392,52 +430,42 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -469,10 +497,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
@@ -481,52 +509,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -879,7 +916,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -894,52 +931,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="30"/>
+      <c r="F1" s="32"/>
       <c r="G1" s="8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="39"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="20" t="s">
+      <c r="A2" s="42"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="26">
+      <c r="B3" s="33">
         <v>30</v>
       </c>
       <c r="C3" s="6">
         <v>30</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="6">
@@ -953,29 +990,29 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="34"/>
-      <c r="B4" s="31"/>
+      <c r="A4" s="37"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="6">
         <v>50</v>
       </c>
-      <c r="D4" s="23"/>
+      <c r="D4" s="27"/>
       <c r="E4" s="6">
         <v>72.48</v>
       </c>
       <c r="F4" s="6">
-        <v>69.25</v>
+        <v>70.09</v>
       </c>
       <c r="G4" s="3">
-        <v>79.94</v>
+        <v>79.7</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="34"/>
-      <c r="B5" s="31"/>
+      <c r="A5" s="37"/>
+      <c r="B5" s="34"/>
       <c r="C5" s="4">
         <v>70</v>
       </c>
-      <c r="D5" s="23"/>
+      <c r="D5" s="27"/>
       <c r="E5" s="4">
         <v>55.79</v>
       </c>
@@ -983,18 +1020,18 @@
         <v>63.24</v>
       </c>
       <c r="G5" s="10">
-        <v>58.91</v>
+        <v>58.83</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="34"/>
-      <c r="B6" s="31">
+      <c r="A6" s="37"/>
+      <c r="B6" s="34">
         <v>50</v>
       </c>
       <c r="C6" s="5">
         <v>30</v>
       </c>
-      <c r="D6" s="23"/>
+      <c r="D6" s="27"/>
       <c r="E6" s="5">
         <v>70.959999999999994</v>
       </c>
@@ -1002,33 +1039,33 @@
         <v>69.040000000000006</v>
       </c>
       <c r="G6" s="9">
-        <v>74.7</v>
+        <v>74.56</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="34"/>
-      <c r="B7" s="31"/>
+      <c r="A7" s="37"/>
+      <c r="B7" s="34"/>
       <c r="C7" s="6">
         <v>50</v>
       </c>
-      <c r="D7" s="23"/>
+      <c r="D7" s="27"/>
       <c r="E7" s="6">
         <v>64.760000000000005</v>
       </c>
       <c r="F7" s="6">
-        <v>69.349999999999994</v>
+        <v>68.69</v>
       </c>
       <c r="G7" s="3">
-        <v>70.55</v>
+        <v>70.28</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="34"/>
-      <c r="B8" s="31"/>
+      <c r="A8" s="37"/>
+      <c r="B8" s="34"/>
       <c r="C8" s="4">
         <v>70</v>
       </c>
-      <c r="D8" s="23"/>
+      <c r="D8" s="27"/>
       <c r="E8" s="4">
         <v>68.2</v>
       </c>
@@ -1040,14 +1077,14 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="34"/>
-      <c r="B9" s="31">
+      <c r="A9" s="37"/>
+      <c r="B9" s="34">
         <v>70</v>
       </c>
       <c r="C9" s="5">
         <v>30</v>
       </c>
-      <c r="D9" s="23"/>
+      <c r="D9" s="27"/>
       <c r="E9" s="5">
         <v>73.39</v>
       </c>
@@ -1059,12 +1096,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="34"/>
-      <c r="B10" s="31"/>
+      <c r="A10" s="37"/>
+      <c r="B10" s="34"/>
       <c r="C10" s="6">
         <v>50</v>
       </c>
-      <c r="D10" s="23"/>
+      <c r="D10" s="27"/>
       <c r="E10" s="6">
         <v>67.53</v>
       </c>
@@ -1072,16 +1109,16 @@
         <v>64.23</v>
       </c>
       <c r="G10" s="3">
-        <v>76.03</v>
+        <v>75.84</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="34"/>
-      <c r="B11" s="31"/>
+      <c r="A11" s="37"/>
+      <c r="B11" s="34"/>
       <c r="C11" s="4">
         <v>70</v>
       </c>
-      <c r="D11" s="23"/>
+      <c r="D11" s="27"/>
       <c r="E11" s="4">
         <v>68.459999999999994</v>
       </c>
@@ -1093,138 +1130,168 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="34"/>
-      <c r="B12" s="31">
+      <c r="A12" s="37"/>
+      <c r="B12" s="34">
         <v>100</v>
       </c>
       <c r="C12" s="5">
         <v>30</v>
       </c>
-      <c r="D12" s="23"/>
+      <c r="D12" s="27"/>
       <c r="E12" s="5">
         <v>76.52</v>
       </c>
       <c r="F12" s="6">
-        <v>73.39</v>
+        <v>74.069999999999993</v>
       </c>
       <c r="G12" s="3">
         <v>88.24</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="34"/>
-      <c r="B13" s="31"/>
+      <c r="A13" s="37"/>
+      <c r="B13" s="34"/>
       <c r="C13" s="6">
         <v>50</v>
       </c>
-      <c r="D13" s="23"/>
+      <c r="D13" s="27"/>
       <c r="E13" s="6">
         <v>76.37</v>
       </c>
       <c r="F13" s="6">
-        <v>71.58</v>
+        <v>72.34</v>
       </c>
       <c r="G13" s="3">
         <v>74.33</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="35"/>
-      <c r="B14" s="32"/>
+      <c r="A14" s="38"/>
+      <c r="B14" s="35"/>
       <c r="C14" s="7">
         <v>70</v>
       </c>
-      <c r="D14" s="24"/>
-      <c r="E14" s="6">
+      <c r="D14" s="23"/>
+      <c r="E14" s="7">
         <v>74.53</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="7">
         <v>73.209999999999994</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="18">
         <v>83.96</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="25">
+      <c r="B15" s="26">
         <v>30</v>
       </c>
-      <c r="C15" s="25">
+      <c r="C15" s="24">
         <v>30</v>
       </c>
-      <c r="D15" s="13">
+      <c r="D15" s="6">
         <v>1E-3</v>
       </c>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="17"/>
+      <c r="E15" s="1">
+        <v>81.17</v>
+      </c>
+      <c r="F15" s="6">
+        <v>77.03</v>
+      </c>
+      <c r="G15" s="17">
+        <v>74.72</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="28"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="14">
+      <c r="A16" s="30"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="6">
         <v>0.01</v>
       </c>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="18"/>
+      <c r="E16" s="1">
+        <v>79.44</v>
+      </c>
+      <c r="F16" s="6">
+        <v>75.73</v>
+      </c>
+      <c r="G16" s="17">
+        <v>81.7</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="28"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="14">
+      <c r="A17" s="30"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="4">
         <v>0.1</v>
       </c>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="18"/>
+      <c r="E17" s="1">
+        <v>79.260000000000005</v>
+      </c>
+      <c r="F17" s="6">
+        <v>75.97</v>
+      </c>
+      <c r="G17" s="17">
+        <v>79.86</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="28"/>
-      <c r="B18" s="22">
+      <c r="A18" s="30"/>
+      <c r="B18" s="28">
         <v>100</v>
       </c>
-      <c r="C18" s="22">
+      <c r="C18" s="21">
         <v>30</v>
       </c>
-      <c r="D18" s="14">
+      <c r="D18" s="6">
         <v>1E-3</v>
       </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="18"/>
+      <c r="E18" s="14">
+        <v>79.03</v>
+      </c>
+      <c r="F18" s="13">
+        <v>76.47</v>
+      </c>
+      <c r="G18" s="16">
+        <v>82.89</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="28"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="14">
+      <c r="A19" s="30"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="6">
         <v>0.01</v>
       </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="18"/>
+      <c r="E19" s="1">
+        <v>75.099999999999994</v>
+      </c>
+      <c r="F19" s="15">
+        <v>72.900000000000006</v>
+      </c>
+      <c r="G19" s="17">
+        <v>87.7</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="29"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="15">
+      <c r="A20" s="31"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="19">
         <v>0.1</v>
       </c>
-      <c r="E20" s="12">
-        <v>73.64</v>
-      </c>
-      <c r="F20" s="12">
-        <v>75</v>
-      </c>
-      <c r="G20" s="19">
-        <v>85.83</v>
+      <c r="E20" s="19">
+        <v>81.03</v>
+      </c>
+      <c r="F20" s="19">
+        <v>76.92</v>
+      </c>
+      <c r="G20" s="20">
+        <v>81.540000000000006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>